<commit_message>
Update new testcase change password after login and adding new testcase in the excel file
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\Software Testing_QA Atomation\Manual Software Testing\Meine eigene Arbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32300C04-BDEA-4782-B33F-BF9D0CE78537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F08D1-D4BC-4F07-AAD4-83F341848AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
   <si>
     <t>Project name</t>
   </si>
@@ -701,110 +701,131 @@
     <t>TC_LiF_008</t>
   </si>
   <si>
-    <t xml:space="preserve">A1. Click on "My Account" Dropmenu
+    <t>TC_LiF_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the password after log in </t>
+  </si>
+  <si>
+    <t>Verify the Login functionality across all supported browsers</t>
+  </si>
+  <si>
+    <t>A1. Log in user in all supported browsers (Chrome, Firefox, Edge)</t>
+  </si>
+  <si>
+    <t>E1. User get logged in in all supported browsers (Chrome, Firefox, Edge)</t>
+  </si>
+  <si>
+    <t>Verify the availability and functionality of the "Forgotten Password" link</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. Upon clicking the link, the user is taken to the "Forgot Your Password" page</t>
+  </si>
+  <si>
+    <t>Log in user using keyboard keys (Tab and Enter)</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Use the Tab key to navigate to the E-Mail Address field, and enter a valid email address
+A4. Use the Tab key to navigate to the password field, and enter a valid password
+A5. Use the Tab key to navigate to the login button, and click on it</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. -
+E4. -
+E5. The user is successfully logged in and is redirected to the "My Account" page</t>
+  </si>
+  <si>
+    <t>Ensure the placeholder text in all input fields matches the expected values</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Verify that the E-Mail Address and Password input fields on the Login page display the correct placeholder text</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Click on the "Forgotten Password" link on the Login page</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. The placeholder text appears in all input fields as expected</t>
+  </si>
+  <si>
+    <t>Check the visibility of the password text</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Enter any text into the password field</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. Ensure that the characters entered in the Password field are hidden (e.g., shown as dots or asterisks)</t>
+  </si>
+  <si>
+    <t>TC_LiF_010</t>
+  </si>
+  <si>
+    <t>TC_LiF_011</t>
+  </si>
+  <si>
+    <t>TC_LiF_012</t>
+  </si>
+  <si>
+    <t>TC_LiF_013</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
 A2. Click on "Login" Button
 A3. Under "Returning Customer", enter a valid email address and a valid password
 A4. Click on "Login"
 A5. Choose "Password" from the right-hand menu.
 A6. Modify the password and click the "Continue" button
 A7. Click on "Logout", then click "Login" at the right-side
-A8. Log in with the old password
-A9. Log in with the new password
-</t>
+A8. Log in with the old password</t>
   </si>
   <si>
     <t>E1. Drop down menu will be displayed
 E2. User is redirected to the "Login" page
 E3. -
 E4. The user is successfully logged in and is redirected to the "My Account" page
-E5. User is redirected to the "Password" page
+E5. User is redirected to the "Change Password" page
 E6. After updating the password, the user should be redirected to the "My Account" page, and a success message should appear: "Success: Your password has been successfully updated"
 A7. The user will be taken to the "Account Logout" page, then to the "Login" page
-A8. The user will not be able to login and an error message " Warning: No match for E-Mail Address and/or Password" will appear
-A9. The user logs in successfully and is directed to the "My Account" page</t>
-  </si>
-  <si>
-    <t>TC_LiF_009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change the password after log in </t>
-  </si>
-  <si>
-    <t>Verify the Login functionality across all supported browsers</t>
-  </si>
-  <si>
-    <t>A1. Log in user in all supported browsers (Chrome, Firefox, Edge)</t>
-  </si>
-  <si>
-    <t>E1. User get logged in in all supported browsers (Chrome, Firefox, Edge)</t>
-  </si>
-  <si>
-    <t>Verify the availability and functionality of the "Forgotten Password" link</t>
-  </si>
-  <si>
-    <t>E1. Drop down menu will be displayed
-E2. User is redirected to the "Login" page
-E3. Upon clicking the link, the user is taken to the "Forgot Your Password" page</t>
-  </si>
-  <si>
-    <t>Log in user using keyboard keys (Tab and Enter)</t>
+A8. The user will not be able to login and an error message " Warning: No match for E-Mail Address and/or Password" will appear</t>
   </si>
   <si>
     <t>A1. Click on "My Account" Dropmenu
 A2. Click on "Login" Button
-A3. Use the Tab key to navigate to the E-Mail Address field, and enter a valid email address
-A4. Use the Tab key to navigate to the password field, and enter a valid password
-A5. Use the Tab key to navigate to the login button, and click on it</t>
+A3. Under "Returning Customer", enter a valid email address and a valid password
+A4. Click on "Login"
+A5. Choose "Password" from the right-hand menu.
+A6. Enter a new password in the "Password" field and a different password in the "Password Confirm" field
+A7. Click on "Continue"</t>
   </si>
   <si>
     <t>E1. Drop down menu will be displayed
 E2. User is redirected to the "Login" page
 E3. -
-E4. -
-E5. The user is successfully logged in and is redirected to the "My Account" page</t>
-  </si>
-  <si>
-    <t>Ensure the placeholder text in all input fields matches the expected values</t>
-  </si>
-  <si>
-    <t>A1. Click on "My Account" Dropmenu
-A2. Click on "Login" Button
-A3. Verify that the E-Mail Address and Password input fields on the Login page display the correct placeholder text</t>
-  </si>
-  <si>
-    <t>A1. Click on "My Account" Dropmenu
-A2. Click on "Login" Button
-A3. Click on the "Forgotten Password" link on the Login page</t>
-  </si>
-  <si>
-    <t>E1. Drop down menu will be displayed
-E2. User is redirected to the "Login" page
-E3. The placeholder text appears in all input fields as expected</t>
-  </si>
-  <si>
-    <t>Check the visibility of the password text</t>
-  </si>
-  <si>
-    <t>A1. Click on "My Account" Dropmenu
-A2. Click on "Login" Button
-A3. Enter any text into the password field</t>
-  </si>
-  <si>
-    <t>E1. Drop down menu will be displayed
-E2. User is redirected to the "Login" page
-E3. Ensure that the characters entered in the Password field are hidden (e.g., shown as dots or asterisks)</t>
-  </si>
-  <si>
-    <t>TC_LiF_010</t>
-  </si>
-  <si>
-    <t>TC_LiF_011</t>
-  </si>
-  <si>
-    <t>TC_LiF_012</t>
-  </si>
-  <si>
-    <t>TC_LiF_013</t>
+E4. The user is successfully logged in and is redirected to the "My Account" page
+E5. User is redirected to the "Change Password" page
+E6. -
+A7. The user is not allowed to proceed and an error message is displayed indicating that the passwords do not match. Error message: Password confirmation does not match password!</t>
+  </si>
+  <si>
+    <t>Change Password After Login (New Password and Confirmation Must Match)</t>
+  </si>
+  <si>
+    <t>TC_LiF_014</t>
   </si>
 </sst>
 </file>
@@ -1865,24 +1886,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2631,10 +2652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
-  <dimension ref="A2:F29"/>
+  <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2837,16 +2858,16 @@
         <v>71</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2857,16 +2878,16 @@
         <v>71</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2877,41 +2898,41 @@
         <v>71</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E19" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>167</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>71</v>
@@ -2931,7 +2952,7 @@
     </row>
     <row r="22" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>71</v>
@@ -2949,52 +2970,65 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="39" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="34" t="s">
+        <v>174</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="E24" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="33"/>
@@ -3023,6 +3057,13 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3153,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07D175B-1EC3-4CE1-9106-5596F0863752}">
   <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding new test cases to Add To Cart Functionality and adding new test to Login test
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F08D1-D4BC-4F07-AAD4-83F341848AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4572E-2AB3-4243-9BC3-162CDD18614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Add to cart" sheetId="3" r:id="rId3"/>
-    <sheet name="Logout" sheetId="1" r:id="rId4"/>
-    <sheet name="Product Display Page" sheetId="5" r:id="rId5"/>
+    <sheet name="Product Display Page" sheetId="5" r:id="rId3"/>
+    <sheet name="Add to cart" sheetId="3" r:id="rId4"/>
+    <sheet name="Logout" sheetId="1" r:id="rId5"/>
     <sheet name="Checkout" sheetId="6" r:id="rId6"/>
     <sheet name="Order History" sheetId="8" r:id="rId7"/>
   </sheets>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="192">
   <si>
     <t>Project name</t>
   </si>
@@ -826,6 +826,49 @@
   </si>
   <si>
     <t>TC_LiF_014</t>
+  </si>
+  <si>
+    <t>TC_ATC_004</t>
+  </si>
+  <si>
+    <t>TS_004 Add To Cart Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add product to cart from product display page </t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Product Name: iMac</t>
+  </si>
+  <si>
+    <t>A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Add to Cart" button on the product display page
+A5. Click on the "Shopping Cart" link within the success message</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
+E5. The shopping cart page opens, showing the newly added product</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+At least one product exists in the system</t>
+  </si>
+  <si>
+    <t>Add product to cart from the  Wish List</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+The User is logged in to his account</t>
+  </si>
+  <si>
+    <t>A1. Click on Wish List on the header option</t>
   </si>
 </sst>
 </file>
@@ -897,7 +940,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -992,11 +1035,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1110,6 +1164,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2654,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3076,11 +3133,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
-  <dimension ref="A2:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3088,12 +3159,12 @@
     <col min="1" max="1" width="27.265625" customWidth="1"/>
     <col min="2" max="2" width="33.46484375" customWidth="1"/>
     <col min="3" max="3" width="32.19921875" customWidth="1"/>
-    <col min="4" max="5" width="30.9296875" customWidth="1"/>
-    <col min="6" max="6" width="38.265625" customWidth="1"/>
+    <col min="4" max="6" width="30.9296875" customWidth="1"/>
+    <col min="7" max="7" width="38.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:6" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:7" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3103,7 +3174,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3113,7 +3184,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3123,7 +3194,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3133,7 +3204,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3143,7 +3214,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3153,8 +3224,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:6" ht="70.150000000000006" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:7" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -3170,17 +3241,52 @@
       <c r="E11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="176.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="38"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+    <row r="12" spans="1:7" ht="221.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3190,7 +3296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07D175B-1EC3-4CE1-9106-5596F0863752}">
   <dimension ref="A2:F35"/>
   <sheetViews>
@@ -3651,20 +3757,6 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding Add To Cart test cases
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4572E-2AB3-4243-9BC3-162CDD18614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDA594-4936-41E2-8065-0463AEFD0903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="213">
   <si>
     <t>Project name</t>
   </si>
@@ -834,9 +834,6 @@
     <t>TS_004 Add To Cart Functionality</t>
   </si>
   <si>
-    <t xml:space="preserve">Add product to cart from product display page </t>
-  </si>
-  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -850,32 +847,138 @@
 A5. Click on the "Shopping Cart" link within the success message</t>
   </si>
   <si>
-    <t>E1. -
+    <t>The User is on the homepage of the application
+At least one product exists in the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+E1. -
 E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
 E3. The product details page opens for the selected product
 E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
 E5. The shopping cart page opens, showing the newly added product</t>
   </si>
   <si>
+    <t>A1. Click on the "Wish List" option in the website header
+A2. Under the "Returning Customer" section, enter a valid email address and a valid password
+A3. Click on "Login"
+A4. Click the "Add to Cart" icon under the "Action" column on the Wish List page
+A5. Click on the "Shopping Cart" option in the website header</t>
+  </si>
+  <si>
+    <t>E1. The Login page is displayed
+E2. -
+E3. The user is successfully logged in and redirected to the Wish List page
+E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!”  
+E5. The Shopping Cart page is displayed, showing the added product</t>
+  </si>
+  <si>
+    <t>TC_ATC_001</t>
+  </si>
+  <si>
+    <t>TC_ATC_002</t>
+  </si>
+  <si>
+    <t>TC_ATC_003</t>
+  </si>
+  <si>
+    <t>The user is on the homepage of the application
+The user is registered with a valid email and password
+The user has previously added at least one product to their Wish List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add product to cart from Product Detail Page </t>
+  </si>
+  <si>
+    <t>Add product to cart from Search Result</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
+E4. An extended mini-cart box is displayed
+E5. The Shopping Cart page is displayed, showing the added product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on Add to Cart in the search  result
+A4. Click on the black cart button (cart icon) displayed on the search results page
+A5. Click on "View Cart" in the extended box
+</t>
+  </si>
+  <si>
+    <t>Add Product to Cart from Featured Section on Homepage</t>
+  </si>
+  <si>
     <t>The User is on the homepage of the application
-At least one product exists in the system</t>
-  </si>
-  <si>
-    <t>Add product to cart from the  Wish List</t>
+At least one product is displayed in the Featured section
+The product is available (in stock and can be added to cart)</t>
+  </si>
+  <si>
+    <t>A1. Click on the "Add to Cart" button for one of the products displayed under the "Featured" section on the homepage
+A2. Click on the "Shopping Cart" icon in the website header</t>
+  </si>
+  <si>
+    <t>E1. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!”
+E2. The Shopping Cart page is displayed, showing the product that was added from the Featured section</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>TC_ATC_005</t>
+  </si>
+  <si>
+    <t>Verify “Add to Cart” Functionality Across Supported Web Environments</t>
   </si>
   <si>
     <t>The User is on the homepage of the application
-The User is logged in to his account</t>
-  </si>
-  <si>
-    <t>A1. Click on Wish List on the header option</t>
+At least one product exists in the system
+Supported environments are defined</t>
+  </si>
+  <si>
+    <t>A1. Open the website in each supported web environment (e.g., Chrome, Firefox, Edge)
+A2. Navigate to a product (e.g., via Featured section or Search)
+A3. Click on the "Add to Cart" button for the selected product
+A4. Open the Shopping Cart (via header or success message link)</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. -
+E3. The product is successfully added to the cart and a success message is displayed
+E4. The cart reflects the correct product and quantity</t>
+  </si>
+  <si>
+    <t>Add product to cart from Wish List</t>
+  </si>
+  <si>
+    <t>Add Product to Cart via Product Comparison Page</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+The user has previously added at least one product to the comparison list</t>
+  </si>
+  <si>
+    <t>A1. Hover the mouse over any top menu option, such as "Desktops", "Laptops &amp; Notebooks", or "Components"
+A2. Click on "Show All" under the hovered menu option
+A3. Click on the "Product compare" displayed on the page
+A4. From the Product Comparison page, click "Add to Cart" for your preferred product
+A5. In the success message, click the "Shopping Cart" link</t>
+  </si>
+  <si>
+    <t>E1. The corresponding dropdown submenu is displayed
+E2. The user is directed to the subcategory of the search product
+E3. The user is redirected to the Product Comparison page showing the selected items for comparison
+E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
+E5. The Shopping Cart page is displayed, showing the added product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +1018,14 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1050,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1166,6 +1277,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2711,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3148,9 +3268,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -3159,8 +3279,10 @@
     <col min="1" max="1" width="27.265625" customWidth="1"/>
     <col min="2" max="2" width="33.46484375" customWidth="1"/>
     <col min="3" max="3" width="32.19921875" customWidth="1"/>
-    <col min="4" max="6" width="30.9296875" customWidth="1"/>
-    <col min="7" max="7" width="38.265625" customWidth="1"/>
+    <col min="4" max="4" width="33.9296875" customWidth="1"/>
+    <col min="5" max="5" width="38.46484375" customWidth="1"/>
+    <col min="6" max="6" width="30.9296875" customWidth="1"/>
+    <col min="7" max="7" width="49.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3242,56 +3364,153 @@
         <v>18</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="221.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12" s="35" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="38" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>191</v>
+    </row>
+    <row r="14" spans="1:7" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="208.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="38"/>
+      <c r="B15" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update Test cases add to cart form product detail page and wish list
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDA594-4936-41E2-8065-0463AEFD0903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB358D-8967-43EE-BFF9-42DC956DD1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="214">
   <si>
     <t>Project name</t>
   </si>
@@ -972,6 +972,9 @@
 E3. The user is redirected to the Product Comparison page showing the selected items for comparison
 E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
 E5. The Shopping Cart page is displayed, showing the added product</t>
+  </si>
+  <si>
+    <t>TC_ATC_006</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1146,22 +1149,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1275,15 +1267,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3270,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3406,10 +3389,10 @@
       <c r="D13" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="40" t="s">
         <v>202</v>
       </c>
       <c r="G13" s="35" t="s">
@@ -3440,7 +3423,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="208.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="38"/>
+      <c r="A15" s="38" t="s">
+        <v>181</v>
+      </c>
       <c r="B15" s="34" t="s">
         <v>182</v>
       </c>
@@ -3453,16 +3438,16 @@
       <c r="E15" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="35" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="38" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>182</v>
@@ -3476,37 +3461,38 @@
       <c r="E16" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="35" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="35" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updating test case Add to cart from search page results
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB358D-8967-43EE-BFF9-42DC956DD1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCC070-07D9-492B-921A-F9809C606DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -3253,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Working on Register functionality and Updating tescases in the Add to Cart functionality
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCC070-07D9-492B-921A-F9809C606DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652977DC-4729-42BE-A779-B8CF2F89D6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
@@ -956,25 +956,34 @@
     <t>Add Product to Cart via Product Comparison Page</t>
   </si>
   <si>
+    <t>TC_ATC_006</t>
+  </si>
+  <si>
     <t>The User is on the homepage of the application
+The user is registered with a valid email and password
 The user has previously added at least one product to the comparison list</t>
   </si>
   <si>
-    <t>A1. Hover the mouse over any top menu option, such as "Desktops", "Laptops &amp; Notebooks", or "Components"
-A2. Click on "Show All" under the hovered menu option
-A3. Click on the "Product compare" displayed on the page
-A4. From the Product Comparison page, click "Add to Cart" for your preferred product
-A5. In the success message, click the "Shopping Cart" link</t>
-  </si>
-  <si>
-    <t>E1. The corresponding dropdown submenu is displayed
-E2. The user is directed to the subcategory of the search product
-E3. The user is redirected to the Product Comparison page showing the selected items for comparison
-E4. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
-E5. The Shopping Cart page is displayed, showing the added product</t>
-  </si>
-  <si>
-    <t>TC_ATC_006</t>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Under "Returning Customer", enter a valid email address and a valid password
+A4. Click on "Login"
+A5. Hover the mouse over any top menu option, such as "Desktops", "Laptops &amp; Notebooks", or "Components"
+A6. Click on "Show All" under the hovered menu option
+A7. Click on the "Product compare" displayed on the page
+A8. From the Product Comparison page, click "Add to Cart" for your preferred product
+A9. In the success message, click the "Shopping Cart" link</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. -
+E4. The user is successfully logged in and is redirected to the "My Account" page
+E5. The corresponding dropdown submenu is displayed
+E6. The user is directed to the subcategory of the search product
+E7. The user is redirected to the Product Comparison page showing the selected items for comparison
+E8. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
+E9. The Shopping Cart page is displayed, showing the added product</t>
   </si>
 </sst>
 </file>
@@ -2814,8 +2823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3253,8 +3262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3422,7 +3431,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="208.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="38" t="s">
         <v>181</v>
       </c>
@@ -3433,16 +3442,16 @@
         <v>209</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F15" s="40" t="s">
         <v>202</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
@@ -3470,7 +3479,7 @@
     </row>
     <row r="17" spans="1:7" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
First test case of registration functionality
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652977DC-4729-42BE-A779-B8CF2F89D6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1990EED-0851-4C01-B0B7-01D15DDD2F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="215">
   <si>
     <t>Project name</t>
   </si>
@@ -984,6 +984,9 @@
 E7. The user is redirected to the Product Comparison page showing the selected items for comparison
 E8. A success message is displayed confirming the product has been added to the cart: “Success: You have added iMac to your shopping cart!” 
 E9. The Shopping Cart page is displayed, showing the added product</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1046,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,6 +1062,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,7 +1171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1280,6 +1289,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3260,10 +3274,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3277,8 +3291,8 @@
     <col min="7" max="7" width="49.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:7" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3288,7 +3302,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3312,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3308,7 +3322,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3318,7 +3332,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3328,7 +3342,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3338,8 +3352,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:7" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:8" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
         <v>190</v>
       </c>
@@ -3384,8 +3398,11 @@
       <c r="G12" s="35" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H12" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="38" t="s">
         <v>191</v>
       </c>
@@ -3407,8 +3424,11 @@
       <c r="G13" s="35" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H13" s="42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="38" t="s">
         <v>192</v>
       </c>
@@ -3430,8 +3450,11 @@
       <c r="G14" s="35" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H14" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="38" t="s">
         <v>181</v>
       </c>
@@ -3453,8 +3476,9 @@
       <c r="G15" s="35" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H15" s="43"/>
+    </row>
+    <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="38" t="s">
         <v>203</v>
       </c>
@@ -3476,8 +3500,9 @@
       <c r="G16" s="35" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H16" s="43"/>
+    </row>
+    <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
         <v>210</v>
       </c>
@@ -3499,6 +3524,7 @@
       <c r="G17" s="35" t="s">
         <v>207</v>
       </c>
+      <c r="H17" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Working on register page and register page locators
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1990EED-0851-4C01-B0B7-01D15DDD2F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDE797-879C-4D32-880A-AA019A8DA11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="216">
   <si>
     <t>Project name</t>
   </si>
@@ -987,6 +987,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>MyPassword1234</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1294,11 +1297,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2045,48 +2087,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="31" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="0" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="23" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="13" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2391,7 +2434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2415,6 +2458,7 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
+      <c r="E3" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
@@ -2425,6 +2469,9 @@
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
+      <c r="E4" s="44" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
@@ -2435,6 +2482,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
@@ -2445,6 +2493,7 @@
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
+      <c r="E6" s="44"/>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
@@ -2455,6 +2504,7 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
@@ -2465,6 +2515,7 @@
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="1:6" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2837,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3276,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
updating resgistration test via my account
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDE797-879C-4D32-880A-AA019A8DA11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D26A9CC-2A1C-4085-A517-05C9908720A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="217">
   <si>
     <t>Project name</t>
   </si>
@@ -990,6 +990,9 @@
   </si>
   <si>
     <t>MyPassword1234</t>
+  </si>
+  <si>
+    <t>Telefon Feld sollte nur Zahken enthlaten, keine Sonderzeichen oder Bustaben ==&gt; Neuer Test zu implementieren</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1052,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1071,6 +1074,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1174,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1298,49 +1307,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1850,6 +1824,44 @@
         <bottom style="thick">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2093,43 +2105,43 @@
     <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
     <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
     <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="0" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="25" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2434,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2818,8 +2830,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:6" ht="57.4" x14ac:dyDescent="0.5">
+      <c r="A26" s="45" t="s">
+        <v>216</v>
+      </c>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="33"/>

</xml_diff>

<commit_message>
Adding test registration via new customer
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D26A9CC-2A1C-4085-A517-05C9908720A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36535422-5F85-47BB-B935-228BB7F4C32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -2446,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
implementing registration testcase without checking the newsletter option
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36535422-5F85-47BB-B935-228BB7F4C32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AD1B79-B534-4794-8C9E-898F2BD1FD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="218">
   <si>
     <t>Project name</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>Telefon Feld sollte nur Zahken enthlaten, keine Sonderzeichen oder Bustaben ==&gt; Neuer Test zu implementieren</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -2444,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2460,8 +2463,8 @@
     <col min="6" max="6" width="62.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:6" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:7" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2475,7 @@
       <c r="D3" s="29"/>
       <c r="E3" s="44"/>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2496,7 +2499,7 @@
       <c r="D5" s="29"/>
       <c r="E5" s="44"/>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2507,7 +2510,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="44"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2518,7 +2521,7 @@
       <c r="D7" s="29"/>
       <c r="E7" s="44"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2529,8 +2532,8 @@
       <c r="D8" s="29"/>
       <c r="E8" s="44"/>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:6" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:7" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="34" t="s">
         <v>73</v>
       </c>
@@ -2569,8 +2572,11 @@
       <c r="F12" s="35" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G12" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
         <v>74</v>
       </c>
@@ -2589,8 +2595,11 @@
       <c r="F13" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G13" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
         <v>81</v>
       </c>
@@ -2609,8 +2618,11 @@
       <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G14" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="36" t="s">
         <v>84</v>
       </c>
@@ -2629,8 +2641,11 @@
       <c r="F15" s="35" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G15" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="36" t="s">
         <v>88</v>
       </c>
@@ -2649,8 +2664,9 @@
       <c r="F16" s="35" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G16" s="42"/>
+    </row>
+    <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="36" t="s">
         <v>89</v>
       </c>
@@ -2669,8 +2685,9 @@
       <c r="F17" s="35" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G17" s="42"/>
+    </row>
+    <row r="18" spans="1:7" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="36" t="s">
         <v>92</v>
       </c>
@@ -2689,8 +2706,9 @@
       <c r="F18" s="35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G18" s="42"/>
+    </row>
+    <row r="19" spans="1:7" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="36" t="s">
         <v>98</v>
       </c>
@@ -2709,8 +2727,9 @@
       <c r="F19" s="35" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G19" s="42"/>
+    </row>
+    <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36" t="s">
         <v>99</v>
       </c>
@@ -2729,8 +2748,9 @@
       <c r="F20" s="35" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G20" s="42"/>
+    </row>
+    <row r="21" spans="1:7" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="36" t="s">
         <v>100</v>
       </c>
@@ -2749,8 +2769,9 @@
       <c r="F21" s="35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G21" s="42"/>
+    </row>
+    <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="36" t="s">
         <v>102</v>
       </c>
@@ -2769,8 +2790,9 @@
       <c r="F22" s="35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G22" s="42"/>
+    </row>
+    <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="36" t="s">
         <v>120</v>
       </c>
@@ -2789,8 +2811,9 @@
       <c r="F23" s="35" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G23" s="42"/>
+    </row>
+    <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36" t="s">
         <v>124</v>
       </c>
@@ -2809,8 +2832,9 @@
       <c r="F24" s="35" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G24" s="42"/>
+    </row>
+    <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="36" t="s">
         <v>125</v>
       </c>
@@ -2829,8 +2853,9 @@
       <c r="F25" s="35" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="57.4" x14ac:dyDescent="0.5">
+      <c r="G25" s="42"/>
+    </row>
+    <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A26" s="45" t="s">
         <v>216</v>
       </c>
@@ -2840,42 +2865,42 @@
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
@@ -2892,8 +2917,9 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Writing testcases for the product display page functionality
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AD1B79-B534-4794-8C9E-898F2BD1FD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23325102-5420-4C4C-A72E-2CD12BA6CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Register" sheetId="4" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="Register" sheetId="4" r:id="rId2"/>
     <sheet name="Product Display Page" sheetId="5" r:id="rId3"/>
     <sheet name="Add to cart" sheetId="3" r:id="rId4"/>
     <sheet name="Logout" sheetId="1" r:id="rId5"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="229">
   <si>
     <t>Project name</t>
   </si>
@@ -996,6 +996,48 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>TC_PDP_001</t>
+  </si>
+  <si>
+    <t>TS_001 Product Display Page</t>
+  </si>
+  <si>
+    <t>A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results</t>
+  </si>
+  <si>
+    <t>Actual Result (AR)</t>
+  </si>
+  <si>
+    <t>Validate presence of product name, brand, and code on the product detail page</t>
+  </si>
+  <si>
+    <t>A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Check that the product display page shows the product name, brand, and code</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The name, brand, and code of the searched product are correctly displayed on the product display page</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC_PDP_002</t>
+  </si>
+  <si>
+    <t>Verify default quantity is 1 when no minimum quantity is set for the product</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+At least one product exists in the system</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1182,11 +1224,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1313,11 +1366,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="52">
     <dxf>
       <font>
         <b val="0"/>
@@ -1869,6 +1925,189 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2102,49 +2341,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="31" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="45" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="43" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="41" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2446,11 +2697,436 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
+  <dimension ref="A2:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.1328125" customWidth="1"/>
+    <col min="5" max="5" width="58.3984375" customWidth="1"/>
+    <col min="6" max="6" width="63.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:6" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>45748</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:6" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2924,26 +3600,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
-  <dimension ref="A2:F30"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
+  <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.1328125" customWidth="1"/>
-    <col min="5" max="5" width="58.3984375" customWidth="1"/>
-    <col min="6" max="6" width="63.59765625" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="33.3984375" customWidth="1"/>
+    <col min="3" max="3" width="30.1328125" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="5" max="6" width="49.3984375" customWidth="1"/>
+    <col min="7" max="7" width="45.19921875" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:6" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +3630,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2963,7 +3640,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2973,7 +3650,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2983,7 +3660,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2993,7 +3670,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3003,8 +3680,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:6" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:8" ht="20.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -3020,346 +3697,65 @@
       <c r="E11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="38" t="s">
-        <v>70</v>
+      <c r="H11" s="46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="34" t="s">
+        <v>218</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>71</v>
+        <v>219</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>129</v>
+        <v>222</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>130</v>
+        <v>223</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>184</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="95.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>71</v>
+        <v>219</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>96</v>
+        <v>228</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3367,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="E4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3380,6 +3776,7 @@
     <col min="5" max="5" width="38.46484375" customWidth="1"/>
     <col min="6" max="6" width="30.9296875" customWidth="1"/>
     <col min="7" max="7" width="49.46484375" customWidth="1"/>
+    <col min="8" max="8" width="28.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3466,6 +3863,9 @@
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
+      <c r="H11" s="46" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
@@ -3515,7 +3915,7 @@
       <c r="G13" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="41" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more test cases for the Product Display Page
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23325102-5420-4C4C-A72E-2CD12BA6CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC27D7-8F7A-42AD-9E3C-89A2E090EF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="244">
   <si>
     <t>Project name</t>
   </si>
@@ -1001,14 +1001,6 @@
     <t>TC_PDP_001</t>
   </si>
   <si>
-    <t>TS_001 Product Display Page</t>
-  </si>
-  <si>
-    <t>A1.  Enter the name of an existing product into the search text box
-A2. Click on the search icon
-A3. Click on the product image from the displayed search results</t>
-  </si>
-  <si>
     <t>Actual Result (AR)</t>
   </si>
   <si>
@@ -1027,9 +1019,6 @@
 E4. The name, brand, and code of the searched product are correctly displayed on the product display page</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>TC_PDP_002</t>
   </si>
   <si>
@@ -1038,6 +1027,95 @@
   <si>
     <t>The User is on the homepage of the application
 At least one product exists in the system</t>
+  </si>
+  <si>
+    <t>A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Check the quantity text field on the Product Display Page
+A5. Update the quantity by increasing it to more than one and add the product to the cart</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The quantity input field should display the default value "1"
+E5. The quantity should be updated, and the product should be added to the cart without any issues</t>
+  </si>
+  <si>
+    <t>TC_PDP_003</t>
+  </si>
+  <si>
+    <t>TC_PDP_004</t>
+  </si>
+  <si>
+    <t>TC_PDP_005</t>
+  </si>
+  <si>
+    <t>TC_PDP_006</t>
+  </si>
+  <si>
+    <t>TC_PDP_007</t>
+  </si>
+  <si>
+    <t>TS_003 Product Display Page</t>
+  </si>
+  <si>
+    <t>Validate that the product’s minimum quantity is correctly set</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+At least one product exists in the system
+The product must have a minimum quantity configured in the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The User is on the homepage of the application
+At least one product exists in the system
+</t>
+  </si>
+  <si>
+    <t>Product Name: Apple Cinema 30"</t>
+  </si>
+  <si>
+    <t>A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Check the quantity text field on the Product Display Page
+A5. Fill in all the mandatory fields, reduce the quantity to less than 2, and attempt to add the product to the cart
+A6. Click the browser’s Back button to return to the previous page
+A7. Increase the quantity to a value greater than the minimum quantity and click the "Add to Cart" button again</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The default minimum quantity for the product is set to "2" and a message stating "This product has a minimum quantity of 2" is displayed below the Add to Cart button
+E5. The product will not be added to the cart. When clicking on the "Shopping Cart" link in the confirmation message, an error will be displayed: "Minimum order amount for Apple Cinema 30" is 2!"
+E6. User is directed to the previous page "Product Display Page"
+E7. The product should be successfully added to the cart without any error messages and with the entered quantity</t>
+  </si>
+  <si>
+    <t>Verify user can write a product review on the Product Display Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page
+A5. Fill in all required fields for the review (e.g., name, review text, rating)
+A6. Submit the review by clicking the “Submit” button
+</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The Reviews section becomes visible
+E5. -
+E6. The review should be submitted successfully, and a confirmation message should appear "Thank you for your review. It has been submitted to the webmaster for approval."</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1125,6 +1203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,7 +1323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1369,6 +1453,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1925,6 +2015,227 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
         <strike val="0"/>
@@ -2106,227 +2417,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2341,61 +2431,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{921B803E-D03F-40F2-B443-C60645F13B23}" name="Tabelle32" displayName="Tabelle32" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{E0067567-E149-4E36-8D5F-A7EA4F25A381}" name="Spalte1" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{D5ACC9CB-E9A2-4BF9-815B-6463EB8CCA0B}" name="Spalte2" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{0154352F-780A-41EF-AC04-891C28512860}" name="Spalte3" headerRowDxfId="45" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{1726C8D8-7833-4725-AA11-C1C2885C8984}" name="Spalte4" headerRowDxfId="43" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="45" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="43" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="41" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F202CA-5FFF-43BA-B6B9-C174F3F691BB}" name="Tabelle3" displayName="Tabelle3" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{30B8E1B8-537F-4845-ACD6-2894D26F8EAA}" name="Spalte1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7107A602-A7A2-4B71-B6DB-E52AAED436EB}" name="Spalte2" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{24BF606B-66F7-4E82-A04E-065E62E85D3F}" name="Spalte3" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C9813E36-9868-4C80-82D1-B255A10821D8}" name="Spalte4" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3602,10 +3692,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3704,7 +3794,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3712,42 +3802,127 @@
         <v>218</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>186</v>
       </c>
       <c r="E12" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="179.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="B13" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="G12" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="H12" s="41" t="s">
+      <c r="G13" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="315.39999999999998" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="189.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="95.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>220</v>
+      <c r="E15" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3864,7 +4039,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Add more test cases for product Display Page scenario
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC27D7-8F7A-42AD-9E3C-89A2E090EF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF96A4D0-5F24-4FFB-A681-6243BAE9E6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="250">
   <si>
     <t>Project name</t>
   </si>
@@ -1055,9 +1055,6 @@
     <t>TC_PDP_006</t>
   </si>
   <si>
-    <t>TC_PDP_007</t>
-  </si>
-  <si>
     <t>TS_003 Product Display Page</t>
   </si>
   <si>
@@ -1116,6 +1113,42 @@
   </si>
   <si>
     <t>Failed</t>
+  </si>
+  <si>
+    <t>A1. Enter any existing Product name into the Search text box field for which there are no existing reviews
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+The product has no existing reviews</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The "Reviews" tab should display "(0)", indicating no reviews are available and The message "There are no reviews for this product" should be displayed in the reviews section</t>
+  </si>
+  <si>
+    <t>Verify the "Reviews" tab displays "0" when no reviews are available</t>
+  </si>
+  <si>
+    <t>Verify the entered text is valid according to the specified character limit</t>
+  </si>
+  <si>
+    <t>A1. Enter any existing Product name into the Search text box field for which there are no existing reviews
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page
+A5. Fill in all required fields for the review. Under "Your Review" enter text below the minimum limit (&lt;25 characters) or above the maximum limit (&gt;1000 characters)</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The Reviews section becomes visible
+E5. The system should prevent submission and display a validation error message " Warning: Review Text must be between 25 and 1000 characters!"</t>
   </si>
 </sst>
 </file>
@@ -1323,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1458,6 +1491,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3692,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
-  <dimension ref="A2:H18"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3802,7 +3841,7 @@
         <v>218</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>220</v>
@@ -3828,13 +3867,13 @@
         <v>223</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>224</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>226</v>
@@ -3854,25 +3893,25 @@
         <v>228</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="D14" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>235</v>
-      </c>
       <c r="E14" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="F14" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>239</v>
-      </c>
       <c r="H14" s="48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="189.4" thickBot="1" x14ac:dyDescent="0.5">
@@ -3880,56 +3919,79 @@
         <v>229</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>225</v>
       </c>
       <c r="E15" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>241</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>242</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H15" s="49"/>
+    </row>
+    <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
         <v>230</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+        <v>232</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="H16" s="49"/>
+    </row>
+    <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
         <v>231</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="B18" s="34" t="s">
-        <v>233</v>
-      </c>
+      <c r="C17" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="H17" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Working on test case validate product having minimum quantity set
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF96A4D0-5F24-4FFB-A681-6243BAE9E6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD4608-03B9-4052-A5B8-BC4726621269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -3733,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated test cases table
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD4608-03B9-4052-A5B8-BC4726621269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E2D226-CC66-42E8-A53A-B3C4D44E6E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -35,12 +35,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="250">
   <si>
     <t>Project name</t>
   </si>
@@ -986,9 +989,6 @@
 E9. The Shopping Cart page is displayed, showing the added product</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>MyPassword1234</t>
   </si>
   <si>
@@ -1149,6 +1149,9 @@
 E3. The product details page opens for the selected product
 E4. The Reviews section becomes visible
 E5. The system should prevent submission and display a validation error message " Warning: Review Text must be between 25 and 1000 characters!"</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1241,7 +1244,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1356,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1477,8 +1498,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1489,14 +1508,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3254,8 +3284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3266,6 +3296,7 @@
     <col min="4" max="4" width="36.86328125" customWidth="1"/>
     <col min="5" max="5" width="61.6640625" customWidth="1"/>
     <col min="6" max="6" width="62.73046875" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3278,7 +3309,7 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="44"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
@@ -3289,8 +3320,8 @@
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
-      <c r="E4" s="44" t="s">
-        <v>215</v>
+      <c r="E4" s="42" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -3302,7 +3333,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
-      <c r="E5" s="44"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
@@ -3313,7 +3344,7 @@
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
-      <c r="E6" s="44"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
@@ -3324,7 +3355,7 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
-      <c r="E7" s="44"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
@@ -3335,10 +3366,10 @@
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="44"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:7" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E8" s="42"/>
+    </row>
+    <row r="10" spans="1:7" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:7" ht="36.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -3356,6 +3387,9 @@
       </c>
       <c r="F11" s="18" t="s">
         <v>14</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3378,7 +3412,7 @@
         <v>79</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3401,7 +3435,7 @@
         <v>80</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3423,9 +3457,7 @@
       <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="41" t="s">
-        <v>217</v>
-      </c>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="36" t="s">
@@ -3447,7 +3479,7 @@
         <v>86</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3469,7 +3501,7 @@
       <c r="F16" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="49"/>
     </row>
     <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="36" t="s">
@@ -3490,7 +3522,9 @@
       <c r="F17" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="41" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="36" t="s">
@@ -3511,7 +3545,9 @@
       <c r="F18" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="42"/>
+      <c r="G18" s="41" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="36" t="s">
@@ -3532,7 +3568,7 @@
       <c r="F19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="42"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36" t="s">
@@ -3553,7 +3589,9 @@
       <c r="F20" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="41" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="36" t="s">
@@ -3574,7 +3612,9 @@
       <c r="F21" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="50" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="36" t="s">
@@ -3595,7 +3635,7 @@
       <c r="F22" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="42"/>
+      <c r="G22" s="49"/>
     </row>
     <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="36" t="s">
@@ -3616,7 +3656,7 @@
       <c r="F23" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="42"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36" t="s">
@@ -3637,7 +3677,7 @@
       <c r="F24" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="42"/>
+      <c r="G24" s="49"/>
     </row>
     <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="36" t="s">
@@ -3658,11 +3698,11 @@
       <c r="F25" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="42"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
-      <c r="A26" s="45" t="s">
-        <v>216</v>
+      <c r="A26" s="43" t="s">
+        <v>215</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -3733,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3832,159 +3872,159 @@
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="46" t="s">
-        <v>219</v>
+      <c r="H11" s="44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>186</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>184</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="179.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>224</v>
-      </c>
       <c r="D13" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F13" s="34" t="s">
         <v>184</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="315.39999999999998" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="D14" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>234</v>
-      </c>
       <c r="E14" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="F14" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>242</v>
+      <c r="H14" s="51" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="189.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="C15" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="F15" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="H15" s="49"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="E16" s="50" t="s">
         <v>243</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>242</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>184</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="H16" s="49"/>
+        <v>244</v>
+      </c>
+      <c r="H16" s="46"/>
     </row>
     <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>232</v>
-      </c>
       <c r="C17" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>247</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>248</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>184</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="H17" s="49"/>
+        <v>248</v>
+      </c>
+      <c r="H17" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4000,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4100,8 +4140,8 @@
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="46" t="s">
-        <v>219</v>
+      <c r="H11" s="44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4127,7 +4167,7 @@
         <v>187</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4153,7 +4193,7 @@
         <v>189</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4179,7 +4219,7 @@
         <v>196</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4204,7 +4244,9 @@
       <c r="G15" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="43"/>
+      <c r="H15" s="53" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="38" t="s">
@@ -4228,7 +4270,7 @@
       <c r="G16" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="43"/>
+      <c r="H16" s="52"/>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
@@ -4252,7 +4294,7 @@
       <c r="G17" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="H17" s="43"/>
+      <c r="H17" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Completed testcode for testcase review text length outside valid range and optimized test case user can cubmit product review on display page
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E2D226-CC66-42E8-A53A-B3C4D44E6E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9BA1BC-0AF0-482D-A287-F493F5DDFC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="250">
   <si>
     <t>Project name</t>
   </si>
@@ -1137,13 +1137,6 @@
     <t>Verify the entered text is valid according to the specified character limit</t>
   </si>
   <si>
-    <t>A1. Enter any existing Product name into the Search text box field for which there are no existing reviews
-A2. Click on the search icon
-A3. Click on the product image from the displayed search results
-A4. Click on the "Reviews" tab on the Product Display Page
-A5. Fill in all required fields for the review. Under "Your Review" enter text below the minimum limit (&lt;25 characters) or above the maximum limit (&gt;1000 characters)</t>
-  </si>
-  <si>
     <t>E1. -
 E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
 E3. The product details page opens for the selected product
@@ -1152,6 +1145,13 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>A1. Enter any existing Product name into the Search text box field
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page
+A5. Fill in all required fields for the review. Under "Your Name" or "Your Review" enter text below the minimum limit (&lt;25 characters) or above the maximum limit (&gt;1000 characters)</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1506,9 +1506,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2860,7 +2857,7 @@
   <dimension ref="A2:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3284,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3457,7 +3454,7 @@
       <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="48"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="36" t="s">
@@ -3501,7 +3498,7 @@
       <c r="F16" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="49"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="36" t="s">
@@ -3568,7 +3565,7 @@
       <c r="F19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="49"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36" t="s">
@@ -3612,7 +3609,7 @@
       <c r="F21" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="49" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3635,7 +3632,7 @@
       <c r="F22" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="49"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="36" t="s">
@@ -3656,7 +3653,7 @@
       <c r="F23" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="49"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36" t="s">
@@ -3677,7 +3674,7 @@
       <c r="F24" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="49"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="36" t="s">
@@ -3698,7 +3695,7 @@
       <c r="F25" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="49"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A26" s="43" t="s">
@@ -3773,8 +3770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3950,7 +3947,7 @@
       <c r="G14" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="50" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3976,7 +3973,9 @@
       <c r="G15" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="H15" s="41"/>
+      <c r="H15" s="41" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
@@ -3991,7 +3990,7 @@
       <c r="D16" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="46" t="s">
         <v>242</v>
       </c>
       <c r="F16" s="34" t="s">
@@ -4000,7 +3999,7 @@
       <c r="G16" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="H16" s="46"/>
+      <c r="H16" s="47"/>
     </row>
     <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
@@ -4016,15 +4015,17 @@
         <v>224</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>184</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="H17" s="46"/>
+        <v>247</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4040,7 +4041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -4244,8 +4245,8 @@
       <c r="G15" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="53" t="s">
-        <v>249</v>
+      <c r="H15" s="52" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
@@ -4270,7 +4271,7 @@
       <c r="G16" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="52"/>
+      <c r="H16" s="51"/>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
@@ -4294,7 +4295,7 @@
       <c r="G17" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="H17" s="52"/>
+      <c r="H17" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Adding warning for your name field to the test reviews
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9BA1BC-0AF0-482D-A287-F493F5DDFC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FBF195-D84B-4ACE-83E1-2DF039AAFC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -3771,7 +3771,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated login via right menu test
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FBF195-D84B-4ACE-83E1-2DF039AAFC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23325327-1B7D-48F2-9F05-1B6F9BB46971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="250">
   <si>
     <t>Project name</t>
   </si>
@@ -1377,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1525,6 +1525,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2854,10 +2855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
-  <dimension ref="A2:F30"/>
+  <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2868,10 +2869,11 @@
     <col min="4" max="4" width="28.1328125" customWidth="1"/>
     <col min="5" max="5" width="58.3984375" customWidth="1"/>
     <col min="6" max="6" width="63.59765625" customWidth="1"/>
+    <col min="7" max="7" width="29.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:6" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:7" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2883,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2891,7 +2893,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2901,7 +2903,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2911,7 +2913,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2921,7 +2923,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2931,8 +2933,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:6" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:7" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -2951,8 +2953,11 @@
       <c r="F11" s="18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G11" s="19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
         <v>70</v>
       </c>
@@ -2971,8 +2976,11 @@
       <c r="F12" s="35" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G12" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
         <v>72</v>
       </c>
@@ -2991,8 +2999,11 @@
       <c r="F13" s="35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G13" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
         <v>133</v>
       </c>
@@ -3011,8 +3022,11 @@
       <c r="F14" s="35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G14" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="39" t="s">
         <v>137</v>
       </c>
@@ -3031,8 +3045,11 @@
       <c r="F15" s="35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G15" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
         <v>150</v>
       </c>
@@ -3051,8 +3068,11 @@
       <c r="F16" s="35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G16" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
         <v>151</v>
       </c>
@@ -3071,8 +3091,11 @@
       <c r="F17" s="35" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G17" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="39" t="s">
         <v>152</v>
       </c>
@@ -3091,8 +3114,11 @@
       <c r="F18" s="35" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G18" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="34" t="s">
         <v>153</v>
       </c>
@@ -3111,8 +3137,11 @@
       <c r="F19" s="35" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G19" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="34" t="s">
         <v>154</v>
       </c>
@@ -3131,8 +3160,11 @@
       <c r="F20" s="35" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G20" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="39" t="s">
         <v>171</v>
       </c>
@@ -3151,8 +3183,11 @@
       <c r="F21" s="35" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G21" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="34" t="s">
         <v>172</v>
       </c>
@@ -3171,8 +3206,9 @@
       <c r="F22" s="35" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G22" s="53"/>
+    </row>
+    <row r="23" spans="1:7" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="34" t="s">
         <v>173</v>
       </c>
@@ -3191,8 +3227,9 @@
       <c r="F23" s="35" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G23" s="53"/>
+    </row>
+    <row r="24" spans="1:7" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="34" t="s">
         <v>174</v>
       </c>
@@ -3211,8 +3248,9 @@
       <c r="F24" s="35" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G24" s="53"/>
+    </row>
+    <row r="25" spans="1:7" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="39" t="s">
         <v>180</v>
       </c>
@@ -3231,36 +3269,37 @@
       <c r="F25" s="37" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="G25" s="53"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -3770,7 +3809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -4042,7 +4081,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4141,7 +4180,7 @@
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="19" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored login/logout flow test with improved assertions and structured logging
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23325327-1B7D-48F2-9F05-1B6F9BB46971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73577B-4066-487B-9929-EA929B31C281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="250">
   <si>
     <t>Project name</t>
   </si>
@@ -670,26 +670,6 @@
 A6. Click on "Newsletter" in the right-hand menu
 A7. Check the "Newsletter Subscription" option
 A8. Click on "Continue" button on the "Newsletter Subscription" page</t>
-  </si>
-  <si>
-    <t>E1. Drop down menu will be displayed
-E2. User is redirected to the "Login" page
-E3. -
-E4. The user is successfully logged in and is redirected to the "My Account" page
-E5. By clicking on "Wish List" (for example), the user should be redirected to their "Wish List" page
-E6. The user is logged out
-E7. The user should be redirected to the previous page (Wish List)
-E8. The user will be redirected to the "Login" page</t>
-  </si>
-  <si>
-    <t>A1. Click on "My Account" Dropmenu
-A2. Click on "Login" Button
-A3. Under "Returning Customer", enter a valid email address and a valid password
-A4. Click on "Login"
-A5. Select an option on the "My Account" page from either the left-side menu or the right-hand menu.
-A6. Select "Logout" by clicking on the "Logout" button in the right-hand menu or by selecting "Logout" from the "My Account" dropdown menu
-A7. Click the browser's back button
-A8. Click on every button on the page</t>
   </si>
   <si>
     <t>TC_LiF_005</t>
@@ -1152,6 +1132,24 @@
 A3. Click on the product image from the displayed search results
 A4. Click on the "Reviews" tab on the Product Display Page
 A5. Fill in all required fields for the review. Under "Your Name" or "Your Review" enter text below the minimum limit (&lt;25 characters) or above the maximum limit (&gt;1000 characters)</t>
+  </si>
+  <si>
+    <t>A1. Click on "My Account" Dropmenu
+A2. Click on "Login" Button
+A3. Under "Returning Customer", enter a valid email address and a valid password
+A4. Click on "Login"
+A5. Select "Logout" by clicking on the "Logout" button in the right-hand menu or by selecting "Logout" from the "My Account" dropdown menu
+A6. Click the browser's back button
+A7. Click on every button on the page</t>
+  </si>
+  <si>
+    <t>E1. Drop down menu will be displayed
+E2. User is redirected to the "Login" page
+E3. -
+E4. The user is successfully logged in and is redirected to the "My Account" page
+E5. The user is logged out
+E6. The user should be redirected to the previous page (My Account)
+E7. The user will be redirected to the "Login" page</t>
   </si>
 </sst>
 </file>
@@ -2857,8 +2855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2954,7 +2952,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2977,7 +2975,7 @@
         <v>131</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3000,7 +2998,7 @@
         <v>135</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3023,7 +3021,7 @@
         <v>135</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3046,12 +3044,12 @@
         <v>135</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>71</v>
@@ -3069,104 +3067,104 @@
         <v>135</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E19" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="35" t="s">
-        <v>167</v>
-      </c>
       <c r="G19" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>71</v>
@@ -3184,12 +3182,12 @@
         <v>145</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>71</v>
@@ -3201,73 +3199,75 @@
         <v>96</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="53"/>
+        <v>249</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="211.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G23" s="53"/>
     </row>
     <row r="24" spans="1:7" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G24" s="53"/>
     </row>
     <row r="25" spans="1:7" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>96</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G25" s="53"/>
     </row>
@@ -3357,7 +3357,7 @@
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -3425,7 +3425,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3448,7 +3448,7 @@
         <v>79</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3471,7 +3471,7 @@
         <v>80</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3515,7 +3515,7 @@
         <v>86</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3559,7 +3559,7 @@
         <v>106</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3582,7 +3582,7 @@
         <v>95</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3626,7 +3626,7 @@
         <v>110</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3649,7 +3649,7 @@
         <v>113</v>
       </c>
       <c r="G21" s="49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3738,7 +3738,7 @@
     </row>
     <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A26" s="43" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -3903,167 +3903,167 @@
         <v>18</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="B12" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="C12" s="34" t="s">
+      <c r="D12" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>221</v>
-      </c>
       <c r="H12" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="179.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>225</v>
-      </c>
       <c r="F13" s="34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="315.39999999999998" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="D14" s="34" t="s">
+      <c r="E14" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="F14" s="34" t="s">
+      <c r="G14" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="G14" s="35" t="s">
-        <v>237</v>
-      </c>
       <c r="H14" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="189.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="34" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C15" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>239</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>240</v>
-      </c>
       <c r="H15" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B16" s="34" t="s">
-        <v>231</v>
-      </c>
       <c r="C16" s="34" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E16" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="35" t="s">
         <v>242</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>244</v>
       </c>
       <c r="H16" s="47"/>
     </row>
     <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H17" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4175,164 +4175,164 @@
         <v>18</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E12" s="35" t="s">
+      <c r="G12" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="F12" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>187</v>
-      </c>
       <c r="H12" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>193</v>
-      </c>
       <c r="E13" s="35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>184</v>
-      </c>
       <c r="G14" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C15" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="E15" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>213</v>
-      </c>
       <c r="H15" s="52" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C16" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="F16" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="35" t="s">
         <v>199</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>201</v>
       </c>
       <c r="H16" s="51"/>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C17" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="F17" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="35" t="s">
         <v>205</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>207</v>
       </c>
       <c r="H17" s="51"/>
     </row>

</xml_diff>

<commit_message>
Implemented login method separately to make the code more robust and reusable
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73577B-4066-487B-9929-EA929B31C281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45506573-3C46-4611-848A-2E2BC727374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -2856,7 +2856,7 @@
   <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Improve add_to_cart test with structured logging and screenshort naming
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45506573-3C46-4611-848A-2E2BC727374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BEA04-ED7C-42BF-9417-874185F83A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="251">
   <si>
     <t>Project name</t>
   </si>
@@ -1150,6 +1150,9 @@
 E5. The user is logged out
 E6. The user should be redirected to the previous page (My Account)
 E7. The user will be redirected to the "Login" page</t>
+  </si>
+  <si>
+    <t>Not run</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1512,7 +1515,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,7 +1525,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2855,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3227,7 +3228,9 @@
       <c r="F23" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="G23" s="53"/>
+      <c r="G23" s="41" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="247.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="34" t="s">
@@ -3248,7 +3251,9 @@
       <c r="F24" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="53"/>
+      <c r="G24" s="41" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="63.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="39" t="s">
@@ -3269,7 +3274,9 @@
       <c r="F25" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="53"/>
+      <c r="G25" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="33"/>
@@ -3320,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3493,7 +3500,9 @@
       <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="47"/>
+      <c r="G14" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="36" t="s">
@@ -3537,7 +3546,9 @@
       <c r="F16" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="48"/>
+      <c r="G16" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="36" t="s">
@@ -3604,7 +3615,9 @@
       <c r="F19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="48"/>
+      <c r="G19" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36" t="s">
@@ -3648,7 +3661,7 @@
       <c r="F21" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="48" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3671,7 +3684,9 @@
       <c r="F22" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="48"/>
+      <c r="G22" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="36" t="s">
@@ -3692,7 +3707,9 @@
       <c r="F23" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36" t="s">
@@ -3713,7 +3730,9 @@
       <c r="F24" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="48"/>
+      <c r="G24" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="36" t="s">
@@ -3734,7 +3753,9 @@
       <c r="F25" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="48"/>
+      <c r="G25" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A26" s="43" t="s">
@@ -3986,7 +4007,7 @@
       <c r="G14" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="49" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4284,7 +4305,7 @@
       <c r="G15" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="51" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4310,7 +4331,7 @@
       <c r="G16" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="H16" s="51"/>
+      <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
@@ -4334,7 +4355,7 @@
       <c r="G17" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="51"/>
+      <c r="H17" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
refactor: extract reusable success message and cart verification login, added helper method to verify success message and product inclusion
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BEA04-ED7C-42BF-9417-874185F83A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817693FC-7A95-4CAD-8073-C323DD766549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Register" sheetId="4" r:id="rId2"/>
-    <sheet name="Product Display Page" sheetId="5" r:id="rId3"/>
-    <sheet name="Add to cart" sheetId="3" r:id="rId4"/>
+    <sheet name="Add to cart" sheetId="3" r:id="rId3"/>
+    <sheet name="Product Display Page" sheetId="5" r:id="rId4"/>
     <sheet name="Logout" sheetId="1" r:id="rId5"/>
     <sheet name="Checkout" sheetId="6" r:id="rId6"/>
     <sheet name="Order History" sheetId="8" r:id="rId7"/>
@@ -2522,24 +2522,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="24"/>
     <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
     <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2856,7 +2856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -3327,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3827,6 +3827,276 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.265625" customWidth="1"/>
+    <col min="2" max="2" width="33.46484375" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" customWidth="1"/>
+    <col min="4" max="4" width="33.9296875" customWidth="1"/>
+    <col min="5" max="5" width="38.46484375" customWidth="1"/>
+    <col min="6" max="6" width="30.9296875" customWidth="1"/>
+    <col min="7" max="7" width="49.46484375" customWidth="1"/>
+    <col min="8" max="8" width="28.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:8" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>45754</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:8" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" s="51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="H17" s="50"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
@@ -4086,276 +4356,6 @@
       <c r="H17" s="41" t="s">
         <v>214</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
-  <dimension ref="A2:H17"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="27.265625" customWidth="1"/>
-    <col min="2" max="2" width="33.46484375" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" customWidth="1"/>
-    <col min="4" max="4" width="33.9296875" customWidth="1"/>
-    <col min="5" max="5" width="38.46484375" customWidth="1"/>
-    <col min="6" max="6" width="30.9296875" customWidth="1"/>
-    <col min="7" max="7" width="49.46484375" customWidth="1"/>
-    <col min="8" max="8" width="28.19921875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:8" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7">
-        <v>45754</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:8" ht="26.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="216.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>185</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="168" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="180.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="295.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="H15" s="51" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="H16" s="50"/>
-    </row>
-    <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="H17" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
test: implement data-driven login test with dynamic logging and failure tracking
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817693FC-7A95-4CAD-8073-C323DD766549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F4D125-0289-4F39-8847-172FEC3C9490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="252">
   <si>
     <t>Project name</t>
   </si>
@@ -1153,6 +1153,9 @@
   </si>
   <si>
     <t>Not run</t>
+  </si>
+  <si>
+    <t>UI/Frontend-Validierung</t>
   </si>
 </sst>
 </file>
@@ -2522,24 +2525,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2854,10 +2857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2871,8 +2874,8 @@
     <col min="7" max="7" width="29.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:7" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:9" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2882,7 +2885,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2892,7 +2895,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +2905,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2912,7 +2915,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2922,7 +2925,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2932,8 +2935,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:7" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:9" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="38" t="s">
         <v>70</v>
       </c>
@@ -2978,8 +2981,11 @@
       <c r="G12" s="41" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
         <v>72</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" ht="107.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
         <v>133</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="39" t="s">
         <v>137</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="34" t="s">
         <v>148</v>
       </c>
@@ -3830,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
test: updated login/logout test with reusable helper methods
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F4D125-0289-4F39-8847-172FEC3C9490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17953EA2-CCA6-4E0B-A58F-386D119CF1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -2860,7 +2860,7 @@
   <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
minor improvemnets to login flow and helper methods
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17953EA2-CCA6-4E0B-A58F-386D119CF1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6888A0-128A-4AA7-A860-525C877224FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -2860,7 +2860,7 @@
   <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Working on test product minimum quantity is correctly set
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6888A0-128A-4AA7-A860-525C877224FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F753E49-A3CD-4B3D-A513-A2F255B41581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
-    <sheet name="Register" sheetId="4" r:id="rId2"/>
-    <sheet name="Add to cart" sheetId="3" r:id="rId3"/>
-    <sheet name="Product Display Page" sheetId="5" r:id="rId4"/>
+    <sheet name="Add to cart" sheetId="3" r:id="rId2"/>
+    <sheet name="Product Display Page" sheetId="5" r:id="rId3"/>
+    <sheet name="Register" sheetId="4" r:id="rId4"/>
     <sheet name="Logout" sheetId="1" r:id="rId5"/>
     <sheet name="Checkout" sheetId="6" r:id="rId6"/>
     <sheet name="Order History" sheetId="8" r:id="rId7"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="252">
   <si>
     <t>Project name</t>
   </si>
@@ -1215,7 +1215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1255,12 +1255,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1381,7 +1375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1521,11 +1515,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2512,19 +2502,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="25"/>
@@ -2536,13 +2513,26 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="14"/>
     <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
     <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2859,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA37A67-8BE3-4F91-AE62-7CD10E9943D2}">
   <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3330,514 +3320,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
-  <dimension ref="A2:G33"/>
-  <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.53125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.86328125" customWidth="1"/>
-    <col min="5" max="5" width="61.6640625" customWidth="1"/>
-    <col min="6" max="6" width="62.73046875" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:7" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="42"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="42" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="42"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="42"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="31">
-        <v>45783</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="42"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="42"/>
-    </row>
-    <row r="10" spans="1:7" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:7" ht="36.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
-      <c r="A26" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A01C625-E81D-4B26-AC24-6B13DE831A32}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="B15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4040,7 +3527,7 @@
       <c r="G15" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="H15" s="51" t="s">
+      <c r="H15" s="49" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4066,7 +3553,9 @@
       <c r="G16" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="H16" s="50"/>
+      <c r="H16" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
@@ -4090,7 +3579,9 @@
       <c r="G17" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="50"/>
+      <c r="H17" s="47" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4102,12 +3593,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4362,6 +3853,509 @@
       <c r="H17" s="41" t="s">
         <v>214</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
+  <dimension ref="A2:G33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.53125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.86328125" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="62.73046875" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:7" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="31">
+        <v>45783</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="10" spans="1:7" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:7" ht="36.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="164.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="184.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="139.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="128.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="124.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">
+      <c r="A26" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Adding Test cases status
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F753E49-A3CD-4B3D-A513-A2F255B41581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B43962-B921-42C3-A0FF-48FC726E60D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="252">
   <si>
     <t>Project name</t>
   </si>
@@ -3597,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3774,8 +3774,8 @@
       <c r="G14" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>239</v>
+      <c r="H14" s="41" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="189.4" thickBot="1" x14ac:dyDescent="0.5">
@@ -3800,8 +3800,8 @@
       <c r="G15" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="H15" s="41" t="s">
-        <v>214</v>
+      <c r="H15" s="49" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3826,7 +3826,9 @@
       <c r="G16" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="H16" s="47"/>
+      <c r="H16" s="49" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="34" t="s">
@@ -3850,7 +3852,7 @@
       <c r="G17" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="49" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on Test user can submit a review
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B43962-B921-42C3-A0FF-48FC726E60D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD7F74-DB8D-4E0B-8ED1-4A340E419D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -3597,7 +3597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -3870,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updating test writing reviews
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD7F74-DB8D-4E0B-8ED1-4A340E419D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75424B12-177A-463F-BBD1-1A7ADDE8C537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -3597,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3870,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD442017-7FC6-412B-9044-F6533D684D70}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
test(review): Add negative testcase for invalid product reviews
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75424B12-177A-463F-BBD1-1A7ADDE8C537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4B9838-64AF-420C-8FC5-FC92150DF8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="252">
   <si>
     <t>Project name</t>
   </si>
@@ -1032,9 +1032,6 @@
     <t>TC_PDP_005</t>
   </si>
   <si>
-    <t>TC_PDP_006</t>
-  </si>
-  <si>
     <t>TS_003 Product Display Page</t>
   </si>
   <si>
@@ -1095,12 +1092,6 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>A1. Enter any existing Product name into the Search text box field for which there are no existing reviews
-A2. Click on the search icon
-A3. Click on the product image from the displayed search results
-A4. Click on the "Reviews" tab on the Product Display Page</t>
-  </si>
-  <si>
     <t>The User is on the homepage of the application
 The product has no existing reviews</t>
   </si>
@@ -1114,24 +1105,7 @@
     <t>Verify the "Reviews" tab displays "0" when no reviews are available</t>
   </si>
   <si>
-    <t>Verify the entered text is valid according to the specified character limit</t>
-  </si>
-  <si>
-    <t>E1. -
-E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
-E3. The product details page opens for the selected product
-E4. The Reviews section becomes visible
-E5. The system should prevent submission and display a validation error message " Warning: Review Text must be between 25 and 1000 characters!"</t>
-  </si>
-  <si>
     <t>In Progress</t>
-  </si>
-  <si>
-    <t>A1. Enter any existing Product name into the Search text box field
-A2. Click on the search icon
-A3. Click on the product image from the displayed search results
-A4. Click on the "Reviews" tab on the Product Display Page
-A5. Fill in all required fields for the review. Under "Your Name" or "Your Review" enter text below the minimum limit (&lt;25 characters) or above the maximum limit (&gt;1000 characters)</t>
   </si>
   <si>
     <t>A1. Click on "My Account" Dropmenu
@@ -1156,6 +1130,37 @@
   </si>
   <si>
     <t>UI/Frontend-Validierung</t>
+  </si>
+  <si>
+    <t>Verify user cannot submit an Invalid Review</t>
+  </si>
+  <si>
+    <t>The User is on the homepage of the application
+The product has a Review tab
+At least one product exists in the system</t>
+  </si>
+  <si>
+    <t>A1. Enter any existing Product name into the Search text box field for which there are no existing reviews
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page
+A5. Submit the review by clicking the “Submit” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1.  Enter the name of an existing product into the search text box
+A2. Click on the search icon
+A3. Click on the product image from the displayed search results
+A4. Click on the "Reviews" tab on the Product Display Page
+A5. Fill in the required review fields with invalid data (e.g., empty values, below or above allowed length and no rating selected).
+A6. Submit the review by clicking the “Submit” button
+</t>
+  </si>
+  <si>
+    <t>E1. -
+E2. The product search results are displayed based on the entered keyword, and the user is directed to the search results page
+E3. The product details page opens for the selected product
+E4. The Reviews section becomes visible
+E5. The system should prevent submission and display a validation error message "Warning: Review Name must be between 3 and 25 characters!" or " Warning: Review Text must be between 25 and 1000 characters!" or "Warning: Please select a review rating!"</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1371,11 +1376,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1506,9 +1548,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1517,6 +1556,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1708,6 +1768,227 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
         <strike val="0"/>
@@ -1987,227 +2268,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thick">
           <color auto="1"/>
@@ -2502,37 +2562,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{71900048-9998-40EB-BFE8-61385A63BF23}" name="Tabelle325" displayName="Tabelle325" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{C91C0426-0F88-4D22-BAEC-57636AA3C703}" name="Spalte1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{4C23B0BD-AB14-495E-97B6-53F93AFF54DD}" name="Spalte2" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{1D1A5DB1-49D6-441E-8836-F195C24C47C0}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{71412078-D570-4752-B2AE-E7C48AC1B008}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB729344-C13E-4AA8-8518-F2E981666D64}" name="Tabelle326" displayName="Tabelle326" ref="A3:D8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{0FED7B19-615B-4A29-88A6-23BB95932EE5}" name="Spalte1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{94F0AB30-B9AD-447A-BB2D-9CAF728E24FA}" name="Spalte2" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{1EF33F05-7C17-4582-A162-520A65E4A403}" name="Spalte3" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{38DE2C6F-A28B-4CBA-AB96-4CEB022832FC}" name="Spalte4" headerRowDxfId="23" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDCB5A68-C612-4499-AD26-5CD74D0FF6B2}" name="Tabelle323" displayName="Tabelle323" ref="A3:E8" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="35" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{348A33AC-824C-4239-9CA9-641F1008318A}" name="Spalte1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{AA73FDC6-2375-424F-A521-3159FCAD2C7A}" name="Spalte2" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{C5E8EB8A-71D9-40B8-A90A-546DBC00B2E5}" name="Spalte3" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{E05FD9FE-5901-4193-BA58-245A55E4F3F8}" name="Spalte4" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{35906151-0D9D-4852-B28B-602537A32919}" name="Spalte5" headerRowDxfId="11" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2972,7 +3032,7 @@
         <v>214</v>
       </c>
       <c r="I12" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -3196,10 +3256,10 @@
         <v>96</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G22" s="41" t="s">
         <v>214</v>
@@ -3270,8 +3330,8 @@
       <c r="F25" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="47" t="s">
-        <v>250</v>
+      <c r="G25" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
@@ -3527,8 +3587,8 @@
       <c r="G15" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="H15" s="49" t="s">
-        <v>246</v>
+      <c r="H15" s="48" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="126.4" thickBot="1" x14ac:dyDescent="0.5">
@@ -3553,8 +3613,8 @@
       <c r="G16" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="H16" s="47" t="s">
-        <v>250</v>
+      <c r="H16" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="142.15" thickBot="1" x14ac:dyDescent="0.5">
@@ -3579,8 +3639,8 @@
       <c r="G17" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="47" t="s">
-        <v>250</v>
+      <c r="H17" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3597,8 +3657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3705,7 +3765,7 @@
         <v>215</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>217</v>
@@ -3731,13 +3791,13 @@
         <v>220</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>221</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>223</v>
@@ -3757,22 +3817,22 @@
         <v>225</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="D14" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>231</v>
-      </c>
       <c r="E14" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="G14" s="35" t="s">
         <v>234</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>235</v>
       </c>
       <c r="H14" s="41" t="s">
         <v>214</v>
@@ -3782,78 +3842,76 @@
       <c r="A15" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="B15" s="34" t="s">
-        <v>229</v>
+      <c r="B15" s="49" t="s">
+        <v>228</v>
       </c>
       <c r="C15" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="F15" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="G15" s="50" t="s">
         <v>237</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="H15" s="49" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="34" t="s">
+      <c r="H15" s="51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="226.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="174.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="B16" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="D16" s="34" t="s">
+      <c r="B17" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="D17" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="F16" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G16" s="35" t="s">
+      <c r="H17" s="54" t="s">
         <v>242</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="H17" s="49" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4043,8 +4101,8 @@
       <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="47" t="s">
-        <v>250</v>
+      <c r="G14" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="94.9" thickBot="1" x14ac:dyDescent="0.5">
@@ -4089,8 +4147,8 @@
       <c r="F16" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="47" t="s">
-        <v>250</v>
+      <c r="G16" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4158,8 +4216,8 @@
       <c r="F19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="47" t="s">
-        <v>250</v>
+      <c r="G19" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4204,8 +4262,8 @@
       <c r="F21" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="48" t="s">
-        <v>239</v>
+      <c r="G21" s="47" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4227,8 +4285,8 @@
       <c r="F22" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="47" t="s">
-        <v>250</v>
+      <c r="G22" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="246.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4250,8 +4308,8 @@
       <c r="F23" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="47" t="s">
-        <v>250</v>
+      <c r="G23" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4273,8 +4331,8 @@
       <c r="F24" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="47" t="s">
-        <v>250</v>
+      <c r="G24" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4296,8 +4354,8 @@
       <c r="F25" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="47" t="s">
-        <v>250</v>
+      <c r="G25" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="57.4" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
docs(test-plan): update structure and content based on ISTQB
</commit_message>
<xml_diff>
--- a/Opencart_TestCases.xlsx
+++ b/Opencart_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4B9838-64AF-420C-8FC5-FC92150DF8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4633470-2554-4540-B6E8-DB432A97E1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F4DCA306-7AE1-48AA-909C-D0C335760CF0}"/>
   </bookViews>
@@ -3657,8 +3657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B3FDFA-CB9B-4F2E-A6B7-52211465097F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>